<commit_message>
franklin-201602558 finishing data analysis
</commit_message>
<xml_diff>
--- a/Estadisticas_QualityData.xlsx
+++ b/Estadisticas_QualityData.xlsx
@@ -89,25 +89,25 @@
     <t>mean</t>
   </si>
   <si>
-    <t>14.2235773653431</t>
-  </si>
-  <si>
-    <t>14.8941176457732</t>
-  </si>
-  <si>
-    <t>10.8015559891309</t>
-  </si>
-  <si>
-    <t>12.4416666677185</t>
-  </si>
-  <si>
-    <t>18.8396396404988</t>
-  </si>
-  <si>
-    <t>15.8673611109455</t>
-  </si>
-  <si>
-    <t>18.5421809840019</t>
+    <t>14.2227408704967</t>
+  </si>
+  <si>
+    <t>893.647058823529</t>
+  </si>
+  <si>
+    <t>10.8034562186542</t>
+  </si>
+  <si>
+    <t>746.5</t>
+  </si>
+  <si>
+    <t>1130.37837837838</t>
+  </si>
+  <si>
+    <t>952.041666666667</t>
+  </si>
+  <si>
+    <t>18.5419634233197</t>
   </si>
   <si>
     <t>scale</t>
@@ -116,25 +116,25 @@
     <t>sd</t>
   </si>
   <si>
-    <t>17.5605077761576</t>
-  </si>
-  <si>
-    <t>14.4359713680667</t>
-  </si>
-  <si>
-    <t>14.7287720462388</t>
-  </si>
-  <si>
-    <t>1.38659107320425</t>
-  </si>
-  <si>
-    <t>18.6452392105779</t>
-  </si>
-  <si>
-    <t>19.6426126926407</t>
-  </si>
-  <si>
-    <t>13.758819013673</t>
+    <t>1053.61913665593</t>
+  </si>
+  <si>
+    <t>866.158282042129</t>
+  </si>
+  <si>
+    <t>883.73441756635</t>
+  </si>
+  <si>
+    <t>83.1954643842899</t>
+  </si>
+  <si>
+    <t>1118.71435262794</t>
+  </si>
+  <si>
+    <t>1178.55676143772</t>
+  </si>
+  <si>
+    <t>825.514186196713</t>
   </si>
 </sst>
 </file>

</xml_diff>